<commit_message>
listado de páginas actualizado
</commit_message>
<xml_diff>
--- a/Listado de paginas.xlsx
+++ b/Listado de paginas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>Título de navegación</t>
   </si>
@@ -168,9 +168,6 @@
     <t>8.1</t>
   </si>
   <si>
-    <t>Gestionar mis vídeos</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
@@ -181,6 +178,54 @@
   </si>
   <si>
     <t>Contacto</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Mis comentarios</t>
+  </si>
+  <si>
+    <t>Historial</t>
+  </si>
+  <si>
+    <t>Mis listas de reproducción</t>
+  </si>
+  <si>
+    <t>Vídeos favoritos</t>
+  </si>
+  <si>
+    <t>Vídeos subidos</t>
+  </si>
+  <si>
+    <t>Mis suscripciones</t>
+  </si>
+  <si>
+    <t>Subir vídeo</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>Ajustes de mi espacio</t>
   </si>
 </sst>
 </file>
@@ -529,15 +574,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" customWidth="1"/>
     <col min="3" max="3" width="14.08984375" customWidth="1"/>
     <col min="5" max="5" width="21.453125" customWidth="1"/>
     <col min="6" max="6" width="33.81640625" customWidth="1"/>
@@ -750,23 +795,87 @@
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
otra actualización listado de paginas...
</commit_message>
<xml_diff>
--- a/Listado de paginas.xlsx
+++ b/Listado de paginas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>Título de navegación</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>8.8</t>
+  </si>
+  <si>
+    <t>Modificación de contraseña</t>
+  </si>
+  <si>
+    <t>6.1</t>
   </si>
 </sst>
 </file>
@@ -570,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -754,17 +760,25 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>